<commit_message>
Debugged synGgen, main and experiment automation
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,55 +451,60 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Density</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Temperature</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Alpha</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>ARI</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>NMI</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Purity</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>H_true</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>H_pred</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>F_measure</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>FM</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Generated_Subgraphs</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Predicted_Subgraphs</t>
         </is>
@@ -518,44 +523,47 @@
         <v>4</v>
       </c>
       <c r="D2" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E2" t="n">
         <v>100</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>0.95</v>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>0.03838015322874863</v>
       </c>
       <c r="H2" t="n">
-        <v>0.24</v>
+        <v>0.1836790287493379</v>
       </c>
       <c r="I2" t="n">
-        <v>2.298688570451097</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>2.2772925846689</v>
       </c>
       <c r="K2" t="n">
-        <v>0.07741935483870968</v>
+        <v>0.4138168503036338</v>
       </c>
       <c r="L2" t="n">
-        <v>0.4163331998932265</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [14, 19, 17, 22, 3, 0] - Density: 0.800004
-Subgraph 2 (Nodes): [8, 10, 11, 28] - Density: 1
-Subgraph 3 (Nodes): [25, 9, 23, 16] - Density: 1
-Subgraph 4 (Nodes): [1, 2, 5, 6, 27] - Density: 1
+        <v>0.1813333333333333</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.4220563913348225</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [15, 12, 5] - Density: 1
+Subgraph 2 (Nodes): [25, 13, 18, 6, 1, 17] - Density: 0.799943
+Subgraph 3 (Nodes): [16, 10, 2, 28, 19, 9] - Density: 0.799943
+Subgraph 4 (Nodes): [22, 21, 29, 3, 7] - Density: 0.700048
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 1 2 3 4 5 6 8 9 10 11 12 14 16 17 18 19 20 22 23 25 26 27 28 29 }</t>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Subgraph 1:z { 1 2 3 5 6 7 9 10 12 13 15 16 17 18 19 21 22 24 25 27 28 29 } N: 22 Triangles: 40 Density: 0.0259682</t>
         </is>
       </c>
     </row>
@@ -572,45 +580,49 @@
         <v>5</v>
       </c>
       <c r="D3" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="E3" t="n">
         <v>200</v>
       </c>
-      <c r="E3" t="n">
+      <c r="F3" t="n">
         <v>0.9</v>
       </c>
-      <c r="F3" t="n">
-        <v>-0.04652898873909656</v>
-      </c>
       <c r="G3" t="n">
-        <v>0.04473429443242034</v>
+        <v>0.08587635745920039</v>
       </c>
       <c r="H3" t="n">
-        <v>0.4523809523809524</v>
+        <v>0.309568703370067</v>
       </c>
       <c r="I3" t="n">
-        <v>2.253506988631334</v>
+        <v>0.3809523809523809</v>
       </c>
       <c r="J3" t="n">
-        <v>0.2761954276479391</v>
+        <v>2.477564079328485</v>
       </c>
       <c r="K3" t="n">
-        <v>0.06204906204906205</v>
+        <v>0.4537163391869449</v>
       </c>
       <c r="L3" t="n">
-        <v>0.440291297415552</v>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [17, 18, 28, 48] - Density: 1
-Subgraph 2 (Nodes): [10, 36, 43, 49, 11] - Density: 1
-Subgraph 3 (Nodes): [26, 13, 21, 23] - Density: 1
-Subgraph 4 (Nodes): [35, 45, 37, 38, 41, 20] - Density: 0.800004
-Subgraph 5 (Nodes): [31, 44, 9, 7] - Density: 1
+        <v>0.03875968992248062</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.4584268186918276</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [38, 46, 20, 10, 14] - Density: 1
+Subgraph 2 (Nodes): [41, 0, 42, 21, 18, 23, 43] - Density: 0.857143
+Subgraph 3 (Nodes): [3, 22, 32, 8, 29, 47, 4, 33, 28] - Density: 0.845224
+Subgraph 4 (Nodes): [1, 36, 2, 48, 26] - Density: 1
+Subgraph 5 (Nodes): [25, 49, 31, 39] - Density: 1
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 1 3 4 5 7 9 10 11 12 13 14 15 16 17 18 19 20 21 22 23 24 26 28 30 31 34 35 36 37 38 39 40 41 43 44 45 46 48 49 }</t>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Subgraph 1:z { 0 1 2 3 4 8 9 10 11 13 14 16 18 19 20 21 22 23 24 26 27 28 29 30 32 33 35 36 37 38 40 41 42 43 44 46 47 48 } N: 38 Triangles: 122 Density: 0.0144332
+Subgraph 2:z { 25 31 39 49 } N: 4 Triangles: 4 Density: 1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added k as an input so that we dont have to hardcode it during tests
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,45 +466,60 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>k</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>ARI</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>NMI</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>GNMI</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>FuzzyARI</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Purity</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>H_true</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>H_pred</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>F_measure</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>FM</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Generated_Subgraphs</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Predicted_Subgraphs</t>
         </is>
@@ -532,38 +547,47 @@
         <v>0.95</v>
       </c>
       <c r="G2" t="n">
-        <v>0.03838015322874863</v>
+        <v>0.001</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1836790287493379</v>
+        <v>0.09469922572960095</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3107373603223778</v>
       </c>
       <c r="J2" t="n">
-        <v>2.2772925846689</v>
+        <v>0.3099513282337183</v>
       </c>
       <c r="K2" t="n">
-        <v>0.4138168503036338</v>
+        <v>0.09469922572960096</v>
       </c>
       <c r="L2" t="n">
-        <v>0.1813333333333333</v>
+        <v>0.45</v>
       </c>
       <c r="M2" t="n">
-        <v>0.4220563913348225</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [15, 12, 5] - Density: 1
-Subgraph 2 (Nodes): [25, 13, 18, 6, 1, 17] - Density: 0.799943
-Subgraph 3 (Nodes): [16, 10, 2, 28, 19, 9] - Density: 0.799943
-Subgraph 4 (Nodes): [22, 21, 29, 3, 7] - Density: 0.700048
+        <v>2.270950594454669</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.6098403047164005</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.2314285714285714</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.4429522220587847</v>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [20, 25, 21] - Density: 1
+Subgraph 2 (Nodes): [1, 4, 24, 11, 29, 15] - Density: 0.799943
+Subgraph 3 (Nodes): [10, 7, 2] - Density: 1
+Subgraph 4 (Nodes): [14, 8, 0, 19] - Density: 1
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 1 2 3 5 6 7 9 10 12 13 15 16 17 18 19 21 22 24 25 27 28 29 } N: 22 Triangles: 40 Density: 0.0259682</t>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Subgraph 1:z { 0 1 2 4 6 7 8 10 11 14 15 19 20 21 24 25 29 } N: 17 Triangles: 23 Density: 0.0338178</t>
         </is>
       </c>
     </row>
@@ -589,40 +613,48 @@
         <v>0.9</v>
       </c>
       <c r="G3" t="n">
-        <v>0.08587635745920039</v>
+        <v>0.001</v>
       </c>
       <c r="H3" t="n">
-        <v>0.309568703370067</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>0.3809523809523809</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>2.477564079328485</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4537163391869449</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.03875968992248062</v>
+        <v>0.2340425531914894</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4584268186918276</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [38, 46, 20, 10, 14] - Density: 1
-Subgraph 2 (Nodes): [41, 0, 42, 21, 18, 23, 43] - Density: 0.857143
-Subgraph 3 (Nodes): [3, 22, 32, 8, 29, 47, 4, 33, 28] - Density: 0.845224
-Subgraph 4 (Nodes): [1, 36, 2, 48, 26] - Density: 1
-Subgraph 5 (Nodes): [25, 49, 31, 39] - Density: 1
+        <v>2.526255260617095</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.05357142857142858</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.4023520119691402</v>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [27, 20, 17, 37, 28, 30, 12, 49, 39] - Density: 0.761897
+Subgraph 2 (Nodes): [45, 34, 21, 41, 26] - Density: 1
+Subgraph 3 (Nodes): [0, 7, 40, 43, 44] - Density: 1
+Subgraph 4 (Nodes): [33, 22, 2, 32, 42, 18, 16, 38] - Density: 0.80358
+Subgraph 5 (Nodes): [6, 15, 13, 11, 48, 3, 10, 47, 29] - Density: 0.833321
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 1 2 3 4 8 9 10 11 13 14 16 18 19 20 21 22 23 24 26 27 28 29 30 32 33 35 36 37 38 40 41 42 43 44 46 47 48 } N: 38 Triangles: 122 Density: 0.0144332
-Subgraph 2:z { 25 31 39 49 } N: 4 Triangles: 4 Density: 1</t>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Subgraph 1:z { 0 1 2 3 5 6 7 8 9 10 11 12 13 14 15 16 17 18 19 20 21 22 24 25 26 27 28 29 30 31 32 33 34 35 37 38 39 40 41 42 43 44 45 46 47 48 49 } N: 47 Triangles: 199 Density: 0.0122144</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Seed Selection using K-Truss
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,60 +466,65 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>k</t>
+          <t>norm_k</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
+          <t>k_Truss</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
           <t>ARI</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>NMI</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>GNMI</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>FuzzyARI</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Purity</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>H_true</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>H_pred</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>F_measure</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>FM</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Generated_Subgraphs</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Predicted_Subgraphs</t>
         </is>
@@ -535,7 +540,7 @@
         <v>30</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
         <v>0.6</v>
@@ -550,45 +555,50 @@
         <v>0.001</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1228564115689788</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3928809525692566</v>
+        <v>-0.03777544596012592</v>
       </c>
       <c r="J2" t="n">
-        <v>0.4041116476374215</v>
+        <v>0.1934321414709257</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1228564115689787</v>
+        <v>0.1857457212598542</v>
       </c>
       <c r="L2" t="n">
-        <v>0.391304347826087</v>
+        <v>-0.03777544596012591</v>
       </c>
       <c r="M2" t="n">
-        <v>2.285129631910751</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="N2" t="n">
-        <v>0.5586293734521992</v>
+        <v>1.887918502671133</v>
       </c>
       <c r="O2" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.6500224216483541</v>
       </c>
       <c r="P2" t="n">
-        <v>0.4774717526842808</v>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [10, 14, 8, 26] - Density: 1
-Subgraph 2 (Nodes): [5, 4, 20] - Density: 1
-Subgraph 3 (Nodes): [12, 3, 2, 7, 0] - Density: 1
-Subgraph 4 (Nodes): [28, 16, 17, 9, 22] - Density: 0.700048
+        <v>0.2261904761904762</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.4040610178208843</v>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [1, 0, 16, 19] - Density: 1
+Subgraph 2 (Nodes): [4, 24, 15, 13] - Density: 1
+Subgraph 3 (Nodes): [10, 6, 5, 25, 11, 22] - Density: 0.799943
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 2 3 7 8 9 10 11 12 13 14 15 16 17 22 23 25 26 28 29 } N: 20 Triangles: 21 Density: 0.0184222
-Subgraph 2:z { 4 5 20 } N: 3 Triangles: 1 Density: 1</t>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>--- DEBUG: Seeds Loaded ---
+Total seeds = 2
+Seed 1: { 5 6 10 11 22 25 } | Triangles: 16 | Density: 0.799943
+Seed 2: { 4 13 15 24 } | Triangles: 4 | Density: 1
+Subgraph 1:z { 0 1 2 4 5 6 10 11 13 15 16 17 19 20 22 23 24 25 26 27 } N: 20 Triangles: 25 Density: 0.0219297</t>
         </is>
       </c>
     </row>
@@ -602,10 +612,10 @@
         <v>50</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="E3" t="n">
         <v>200</v>
@@ -617,45 +627,51 @@
         <v>0.001</v>
       </c>
       <c r="H3" t="n">
-        <v>-0.04135692338190108</v>
+        <v>3</v>
       </c>
       <c r="I3" t="n">
-        <v>0.05007327186960253</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>0.08021295050463162</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-0.0413569233819011</v>
+        <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>0.4146341463414634</v>
+        <v>0</v>
       </c>
       <c r="M3" t="n">
-        <v>2.295943021238485</v>
+        <v>0.35</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2811937964320427</v>
+        <v>1.93703267660925</v>
       </c>
       <c r="O3" t="n">
-        <v>0.05889724310776942</v>
+        <v>0</v>
       </c>
       <c r="P3" t="n">
-        <v>0.4214799273318533</v>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [35, 49, 23] - Density: 1
-Subgraph 2 (Nodes): [2, 36, 41, 46, 14, 39] - Density: 0.799943
-Subgraph 3 (Nodes): [44, 40, 31, 32, 26, 30] - Density: 0.799943
-Subgraph 4 (Nodes): [24, 25, 3, 21, 11, 20] - Density: 0.799943
-Subgraph 5 (Nodes): [12, 28, 0] - Density: 1
+        <v>0.1296296296296296</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.5025575614435649</v>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [46, 45, 19, 43, 14, 35, 9, 41, 28, 25, 4, 42, 27, 5] - Density: 0.513739
+Subgraph 2 (Nodes): [36, 8, 33, 40, 11, 48] - Density: 0.549961
+Subgraph 3 (Nodes): [39, 26, 23, 15, 3, 1, 7, 47, 6] - Density: 0.607122
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 1 2 3 5 6 7 9 11 12 13 14 15 17 18 20 21 23 24 25 26 27 28 29 30 31 32 33 35 36 38 39 40 41 42 43 44 46 49 } N: 39 Triangles: 50 Density: 0.00545867</t>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>--- DEBUG: Seeds Loaded ---
+Total seeds = 3
+Seed 1: { 8 11 33 36 40 48 } | Triangles: 11 | Density: 0.549961
+Seed 2: { 4 5 9 14 19 25 27 28 35 41 42 43 45 46 } | Triangles: 187 | Density: 0.513739
+Seed 3: { 1 3 6 7 15 23 26 39 47 } | Triangles: 51 | Density: 0.607122
+Subgraph 1:z { 1 2 3 4 5 6 7 8 9 10 11 14 15 19 20 21 22 23 25 26 27 28 29 30 32 33 34 35 36 38 39 40 41 42 43 44 45 46 47 48 } N: 40 Triangles: 249 Density: 0.0251435</t>
         </is>
       </c>
     </row>
@@ -669,7 +685,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="n">
         <v>0.6</v>
@@ -684,45 +700,50 @@
         <v>0.001</v>
       </c>
       <c r="H4" t="n">
-        <v>0.1228564115689788</v>
+        <v>3</v>
       </c>
       <c r="I4" t="n">
-        <v>0.3928809525692566</v>
+        <v>-0.03777544596012592</v>
       </c>
       <c r="J4" t="n">
-        <v>0.4041116476374215</v>
+        <v>0.1934321414709257</v>
       </c>
       <c r="K4" t="n">
-        <v>0.1228564115689787</v>
+        <v>0.1857457212598542</v>
       </c>
       <c r="L4" t="n">
-        <v>0.391304347826087</v>
+        <v>-0.03777544596012591</v>
       </c>
       <c r="M4" t="n">
-        <v>2.285129631910751</v>
+        <v>0.4166666666666667</v>
       </c>
       <c r="N4" t="n">
-        <v>0.5586293734521992</v>
+        <v>1.887918502671133</v>
       </c>
       <c r="O4" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.6500224216483541</v>
       </c>
       <c r="P4" t="n">
-        <v>0.4774717526842808</v>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [10, 14, 8, 26] - Density: 1
-Subgraph 2 (Nodes): [5, 4, 20] - Density: 1
-Subgraph 3 (Nodes): [12, 3, 2, 7, 0] - Density: 1
-Subgraph 4 (Nodes): [28, 16, 17, 9, 22] - Density: 0.700048
+        <v>0.2261904761904762</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.4040610178208843</v>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [1, 0, 16, 19] - Density: 1
+Subgraph 2 (Nodes): [4, 24, 15, 13] - Density: 1
+Subgraph 3 (Nodes): [10, 6, 5, 25, 11, 22] - Density: 0.799943
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 2 3 7 8 9 10 11 12 13 14 15 16 17 22 23 25 26 28 29 } N: 20 Triangles: 21 Density: 0.0184222
-Subgraph 2:z { 4 5 20 } N: 3 Triangles: 1 Density: 1</t>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>--- DEBUG: Seeds Loaded ---
+Total seeds = 2
+Seed 1: { 5 6 10 11 22 25 } | Triangles: 16 | Density: 0.799943
+Seed 2: { 4 13 15 24 } | Triangles: 4 | Density: 1
+Subgraph 1:z { 0 1 2 4 5 6 10 11 13 15 16 17 19 20 22 23 24 25 26 27 } N: 20 Triangles: 25 Density: 0.0219297</t>
         </is>
       </c>
     </row>
@@ -736,10 +757,10 @@
         <v>50</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7</v>
+        <v>0.45</v>
       </c>
       <c r="E5" t="n">
         <v>200</v>
@@ -751,45 +772,51 @@
         <v>0.001</v>
       </c>
       <c r="H5" t="n">
-        <v>-0.04135692338190108</v>
+        <v>3</v>
       </c>
       <c r="I5" t="n">
-        <v>0.05007327186960253</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.08021295050463162</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>-0.0413569233819011</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>0.4146341463414634</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>2.295943021238485</v>
+        <v>0.35</v>
       </c>
       <c r="N5" t="n">
-        <v>0.2811937964320427</v>
+        <v>1.93703267660925</v>
       </c>
       <c r="O5" t="n">
-        <v>0.05889724310776942</v>
+        <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>0.4214799273318533</v>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Subgraph 1 (Nodes): [35, 49, 23] - Density: 1
-Subgraph 2 (Nodes): [2, 36, 41, 46, 14, 39] - Density: 0.799943
-Subgraph 3 (Nodes): [44, 40, 31, 32, 26, 30] - Density: 0.799943
-Subgraph 4 (Nodes): [24, 25, 3, 21, 11, 20] - Density: 0.799943
-Subgraph 5 (Nodes): [12, 28, 0] - Density: 1
+        <v>0.1296296296296296</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.5025575614435649</v>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>Subgraph 1 (Nodes): [46, 45, 19, 43, 14, 35, 9, 41, 28, 25, 4, 42, 27, 5] - Density: 0.513739
+Subgraph 2 (Nodes): [36, 8, 33, 40, 11, 48] - Density: 0.549961
+Subgraph 3 (Nodes): [39, 26, 23, 15, 3, 1, 7, 47, 6] - Density: 0.607122
 ----------------------------------------------------</t>
         </is>
       </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>Subgraph 1:z { 0 1 2 3 5 6 7 9 11 12 13 14 15 17 18 20 21 23 24 25 26 27 28 29 30 31 32 33 35 36 38 39 40 41 42 43 44 46 49 } N: 39 Triangles: 50 Density: 0.00545867</t>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>--- DEBUG: Seeds Loaded ---
+Total seeds = 3
+Seed 1: { 8 11 33 36 40 48 } | Triangles: 11 | Density: 0.549961
+Seed 2: { 4 5 9 14 19 25 27 28 35 41 42 43 45 46 } | Triangles: 187 | Density: 0.513739
+Seed 3: { 1 3 6 7 15 23 26 39 47 } | Triangles: 51 | Density: 0.607122
+Subgraph 1:z { 1 2 3 4 5 6 7 8 9 10 11 14 15 19 20 21 22 23 25 26 27 28 29 30 32 33 34 35 36 38 39 40 41 42 43 44 45 46 47 48 } N: 40 Triangles: 249 Density: 0.0251435</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed synGgen for gound truth overlapping, fixed MTDS main, getting better rrestuls
</commit_message>
<xml_diff>
--- a/experiment_results.xlsx
+++ b/experiment_results.xlsx
@@ -537,58 +537,59 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0.82</v>
+        <v>0.944</v>
       </c>
       <c r="E2" t="n">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F2" t="n">
-        <v>0.964</v>
+        <v>0.894</v>
       </c>
       <c r="G2" t="n">
         <v>0.001</v>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0003393547039782813</v>
+        <v>0.324</v>
       </c>
       <c r="J2" t="n">
-        <v>0.09060608731467829</v>
+        <v>0.532</v>
       </c>
       <c r="K2" t="n">
-        <v>0.1331655773385458</v>
+        <v>0.381</v>
       </c>
       <c r="L2" t="n">
-        <v>0.0003393547039782842</v>
+        <v>0.324</v>
       </c>
       <c r="M2" t="n">
-        <v>0.3783783783783784</v>
+        <v>0.611</v>
       </c>
       <c r="N2" t="n">
-        <v>1.90424853420901</v>
+        <v>2.062</v>
       </c>
       <c r="O2" t="n">
-        <v>0.303374836086414</v>
+        <v>1.481</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1282051282051282</v>
+        <v>0.314</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.4809870321024526</v>
+        <v>0.541</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>Subgraph 1 (Nodes): [28, 41, 11, 3, 1, 13, 30, 42, 26, 22, 32, 7] - Density: 0.82273
-Subgraph 2 (Nodes): [15, 4, 2, 9] - Density: 1
-Subgraph 3 (Nodes): [5, 37, 38, 12, 31, 19, 16, 27, 0, 21] - Density: 0.808335
+          <t>Subgraph 1 (Nodes): [62, 54, 37, 41, 40, 26, 50] - Density: 1
+Subgraph 2 (Nodes): [35, 66, 18, 25, 33, 11, 36] - Density: 0.857143
+Subgraph 3 (Nodes): [67, 15, 12, 59, 10, 29] - Density: 1
+Subgraph 4 (Nodes): [31, 44, 6, 42, 16, 22, 45, 32, 7] - Density: 0.916647
 ----------------------------------------------------</t>
         </is>
       </c>
@@ -596,10 +597,10 @@
         <is>
           <t>--- DEBUG: Seeds Loaded ---
 Total seeds = 2
-Seed 1: { 2 4 9 15 } | Triangles: 4 | Density: 1
-Seed 2: { 1 3 7 11 13 22 26 28 30 32 41 42 } | Triangles: 181 | Density: 0.82273
-Subgraph 1:z { 0 1 2 3 4 5 7 8 9 11 12 13 14 15 16 18 19 21 22 24 25 26 27 28 29 30 31 32 35 36 37 38 39 41 42 } N: 35 Triangles: 282 Density: 0.0430308
-Subgraph 2:z { 0 1 2 3 4 5 7 8 9 11 12 13 14 15 16 18 19 21 22 24 25 26 27 28 29 30 31 32 35 36 37 38 39 41 42 } N: 35 Triangles: 282 Density: 0.0430308</t>
+Seed 1: { 26 37 40 41 50 54 62 } | Triangles: 35 | Density: 1
+Seed 2: { 10 12 15 29 59 67 } | Triangles: 20 | Density: 1
+Subgraph 1:z { 1 26 37 40 41 48 50 54 62 } N: 9 Triangles: 35 Density: 0.416647
+Subgraph 2:z { 0 6 7 10 12 14 15 16 22 27 29 30 31 32 34 42 44 45 59 63 67 } N: 21 Triangles: 97 Density: 0.0729225</t>
         </is>
       </c>
     </row>
@@ -610,58 +611,58 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C3" t="n">
         <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>0.803</v>
+        <v>0.823</v>
       </c>
       <c r="E3" t="n">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="F3" t="n">
-        <v>0.827</v>
+        <v>0.902</v>
       </c>
       <c r="G3" t="n">
         <v>0.001</v>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I3" t="n">
-        <v>-0.02758020933627357</v>
+        <v>0.021</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1261747596559608</v>
+        <v>0.161</v>
       </c>
       <c r="K3" t="n">
-        <v>0.1398678831193223</v>
+        <v>0.185</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.02758020933627352</v>
+        <v>0.021</v>
       </c>
       <c r="M3" t="n">
-        <v>0.4</v>
+        <v>0.439</v>
       </c>
       <c r="N3" t="n">
-        <v>1.821230188486178</v>
+        <v>1.934</v>
       </c>
       <c r="O3" t="n">
-        <v>0.4689955935892812</v>
+        <v>0.461</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1384615384615385</v>
+        <v>0.223</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.4646832940632596</v>
+        <v>0.471</v>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>Subgraph 1 (Nodes): [9, 38, 28, 44, 47, 23, 31, 22, 15, 1] - Density: 0.808335
-Subgraph 2 (Nodes): [29, 36, 16] - Density: 1
-Subgraph 3 (Nodes): [3, 41, 40, 27, 30, 32, 26, 14, 48, 6, 33] - Density: 0.80607
+          <t>Subgraph 1 (Nodes): [25, 4, 3, 33, 5, 45] - Density: 1
+Subgraph 2 (Nodes): [46, 9, 20, 43, 47, 44, 56, 1, 37] - Density: 0.845224
+Subgraph 3 (Nodes): [21, 51, 0, 42, 26, 16, 2, 50, 19, 8, 39, 11, 32, 22] - Density: 0.813187
 ----------------------------------------------------</t>
         </is>
       </c>
@@ -669,10 +670,10 @@
         <is>
           <t>--- DEBUG: Seeds Loaded ---
 Total seeds = 2
-Seed 1: { 1 9 15 22 23 28 31 38 44 47 } | Triangles: 97 | Density: 0.808335
-Seed 2: { 3 6 14 26 27 30 32 33 40 41 48 } | Triangles: 133 | Density: 0.80607
-Subgraph 1:z { 1 2 3 4 6 7 8 9 11 14 15 16 17 19 21 22 23 26 27 28 29 30 31 32 33 36 37 38 40 41 42 43 44 46 47 48 } N: 36 Triangles: 233 Density: 0.0325852
-Subgraph 2:z { 1 2 3 4 6 7 8 9 11 14 15 16 17 19 21 22 23 26 27 28 29 30 31 32 33 36 37 38 40 41 42 43 44 46 47 48 } N: 36 Triangles: 233 Density: 0.0325852</t>
+Seed 1: { 1 9 20 37 43 44 46 47 56 } | Triangles: 71 | Density: 0.845224
+Seed 2: { 3 4 5 25 33 45 } | Triangles: 20 | Density: 1
+Subgraph 1:z { 0 1 2 3 4 5 8 9 11 16 19 20 21 22 23 24 25 26 27 30 32 33 36 37 39 42 43 44 45 46 47 48 50 51 54 56 57 } N: 37 Triangles: 387 Density: 0.0497287
+Subgraph 2:z { 0 1 2 3 4 5 8 9 11 16 19 20 21 22 23 24 25 26 27 30 32 33 36 37 39 42 43 44 45 46 47 48 50 51 54 56 57 } N: 37 Triangles: 387 Density: 0.0497287</t>
         </is>
       </c>
     </row>
@@ -683,59 +684,60 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
-        <v>0.8159999999999999</v>
+        <v>0.85</v>
       </c>
       <c r="E4" t="n">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="F4" t="n">
-        <v>0.903</v>
+        <v>0.931</v>
       </c>
       <c r="G4" t="n">
         <v>0.001</v>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1099091302466465</v>
+        <v>0.018</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3327710322084793</v>
+        <v>0.09</v>
       </c>
       <c r="K4" t="n">
-        <v>0.406202522178304</v>
+        <v>0.202</v>
       </c>
       <c r="L4" t="n">
-        <v>0.1099091302466464</v>
+        <v>0.018</v>
       </c>
       <c r="M4" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.242</v>
       </c>
       <c r="N4" t="n">
-        <v>2.157124495039615</v>
+        <v>2.518</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4305518670104394</v>
+        <v>0.196</v>
       </c>
       <c r="P4" t="n">
-        <v>0.3181818181818182</v>
+        <v>0.155</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.5209294783053857</v>
+        <v>0.415</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>Subgraph 1 (Nodes): [8, 24, 3] - Density: 1
-Subgraph 2 (Nodes): [9, 40, 28, 12, 25, 30] - Density: 1
-Subgraph 3 (Nodes): [16, 37, 10, 0, 15] - Density: 1
-Subgraph 4 (Nodes): [2, 34, 22, 17, 39, 5, 19] - Density: 0.857143
+          <t>Subgraph 1 (Nodes): [39, 70, 46, 35, 31, 23, 64, 24, 45, 26, 30, 34, 20, 14] - Density: 0.837919
+Subgraph 2 (Nodes): [28, 18, 42, 53, 15, 40, 32, 43, 2, 11, 50, 74, 3, 59] - Density: 0.843412
+Subgraph 3 (Nodes): [10, 17, 44, 60, 5, 38, 41, 63, 25, 72, 36, 8, 67] - Density: 0.853144
+Subgraph 4 (Nodes): [68, 47, 6, 0, 19, 52, 4, 21, 51, 12] - Density: 0.816659
+Subgraph 5 (Nodes): [1, 37, 58, 54, 55, 49, 69, 56, 22, 13] - Density: 0.808335
 ----------------------------------------------------</t>
         </is>
       </c>
@@ -743,8 +745,8 @@
         <is>
           <t>--- DEBUG: Seeds Loaded ---
 Total seeds = 1
-Seed 1: { 3 8 24 } | Triangles: 1 | Density: 1
-Subgraph 1:z { 3 8 24 } N: 3 Triangles: 1 Density: 1</t>
+Seed 1: { 5 8 10 17 25 36 38 41 44 60 63 67 72 } | Triangles: 244 | Density: 0.853144
+Subgraph 1:z { 0 1 2 3 4 5 6 8 10 11 12 13 14 15 17 18 19 20 21 22 23 24 25 26 28 29 30 31 32 33 34 35 36 37 38 39 40 41 42 43 44 45 46 47 49 50 51 52 53 54 55 56 58 59 60 63 64 66 67 68 69 70 72 74 } N: 64 Triangles: 1051 Density: 0.0248179</t>
         </is>
       </c>
     </row>
@@ -755,25 +757,25 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>34</v>
+        <v>141</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
-        <v>0.758</v>
+        <v>0.824</v>
       </c>
       <c r="E5" t="n">
-        <v>126</v>
+        <v>96</v>
       </c>
       <c r="F5" t="n">
-        <v>0.988</v>
+        <v>0.898</v>
       </c>
       <c r="G5" t="n">
         <v>0.001</v>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I5" t="n">
         <v>0</v>
@@ -788,39 +790,32 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0.2916666666666667</v>
+        <v>0.358</v>
       </c>
       <c r="N5" t="n">
-        <v>2.192215752170299</v>
+        <v>1.879</v>
       </c>
       <c r="O5" t="n">
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>0.08</v>
+        <v>0.132</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.4464026907612011</v>
+        <v>0.531</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>Subgraph 1 (Nodes): [9, 32, 26, 8, 28, 3] - Density: 0.799943
-Subgraph 2 (Nodes): [12, 0, 14, 30, 25, 19, 2] - Density: 0.857143
-Subgraph 3 (Nodes): [33, 7, 11, 31, 20, 22] - Density: 0.799943
-Subgraph 4 (Nodes): [24, 21, 4] - Density: 1
+          <t>Subgraph 1 (Nodes): [3, 64, 84, 119, 12, 99, 94, 69, 55, 24, 46, 76, 98, 111, 60, 86, 53, 88, 48, 79, 0, 66, 116, 39, 92, 74, 20, 108, 67, 72, 27, 114, 133, 77, 51, 9, 49, 85, 56, 41, 128, 137] - Density: 0.806918
+Subgraph 2 (Nodes): [17, 130, 91, 58, 96, 131, 106, 80, 59, 134, 135, 62, 21, 26] - Density: 0.813187
+Subgraph 3 (Nodes): [125, 87, 127, 93, 107, 117, 44, 118, 36, 1, 83, 113, 23, 140, 105, 30, 109, 5, 95, 112, 18, 8, 11, 19, 29, 70, 138, 2, 16, 78] - Density: 0.816823
 ----------------------------------------------------</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
           <t>--- DEBUG: Seeds Loaded ---
-Total seeds = 3
-Seed 1: { 7 11 20 22 31 33 } | Triangles: 16 | Density: 0.799943
-Seed 2: { 0 2 12 14 19 25 30 } | Triangles: 30 | Density: 0.857143
-Seed 3: { 3 8 9 26 28 32 } | Triangles: 16 | Density: 0.799943
-Subgraph 1:z { 0 2 3 4 7 8 9 10 11 12 14 19 20 21 22 24 25 26 28 29 30 31 32 33 } N: 24 Triangles: 63 Density: 0.0311196
-Subgraph 2:z { 0 2 3 4 7 8 9 10 11 12 14 19 20 21 22 24 25 26 28 29 30 31 32 33 } N: 24 Triangles: 63 Density: 0.0311196
-Subgraph 3:z { 0 2 3 4 7 8 9 10 11 12 14 19 20 21 22 24 25 26 28 29 30 31 32 33 } N: 24 Triangles: 63 Density: 0.0311196</t>
+Total seeds = 0</t>
         </is>
       </c>
     </row>
@@ -831,65 +826,73 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" t="n">
-        <v>0.869</v>
+        <v>0.858</v>
       </c>
       <c r="E6" t="n">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F6" t="n">
-        <v>0.956</v>
+        <v>0.958</v>
       </c>
       <c r="G6" t="n">
         <v>0.001</v>
       </c>
       <c r="H6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>0.233</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>0.524</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>0.438</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>0.233</v>
       </c>
       <c r="M6" t="n">
-        <v>0.3225806451612903</v>
+        <v>0.5</v>
       </c>
       <c r="N6" t="n">
-        <v>1.953882410687053</v>
+        <v>2.285</v>
       </c>
       <c r="O6" t="n">
-        <v>0</v>
+        <v>0.8110000000000001</v>
       </c>
       <c r="P6" t="n">
-        <v>0.1219512195121951</v>
+        <v>0.1</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.4907751165796443</v>
+        <v>0.528</v>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>Subgraph 1 (Nodes): [1, 15, 34, 9, 16] - Density: 1
-Subgraph 2 (Nodes): [10, 21, 5, 29, 12, 23, 25] - Density: 0.857143
-Subgraph 3 (Nodes): [17, 27, 3, 6, 37, 33, 18, 13, 2] - Density: 0.845224
+          <t>Subgraph 1 (Nodes): [1, 6, 13, 2, 8] - Density: 1
+Subgraph 2 (Nodes): [28, 12, 21, 16, 7] - Density: 1
+Subgraph 3 (Nodes): [25, 18, 22] - Density: 1
+Subgraph 4 (Nodes): [29, 19, 27] - Density: 1
+Subgraph 5 (Nodes): [14, 0, 30, 20] - Density: 1
 ----------------------------------------------------</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
           <t>--- DEBUG: Seeds Loaded ---
-Total seeds = 0</t>
+Total seeds = 3
+Seed 1: { 7 12 16 21 28 } | Triangles: 10 | Density: 1
+Seed 2: { 0 14 20 30 } | Triangles: 4 | Density: 1
+Seed 3: { 1 2 6 8 13 } | Triangles: 10 | Density: 1
+Subgraph 1:z { 0 7 12 14 16 18 19 20 21 22 25 27 28 29 30 } N: 15 Triangles: 16 Density: 0.035166
+Subgraph 2:z { 0 7 12 14 16 18 19 20 21 22 25 27 28 29 30 } N: 15 Triangles: 16 Density: 0.035166
+Subgraph 3:z { 1 2 6 8 13 } N: 5 Triangles: 10 Density: 1</t>
         </is>
       </c>
     </row>

</xml_diff>